<commit_message>
Data columns formulated for personas and removed encodings.
</commit_message>
<xml_diff>
--- a/data/0_Reformated_SOSEC_Code-book_US_November.xlsx
+++ b/data/0_Reformated_SOSEC_Code-book_US_November.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_workspace\_vscode\Universität-Trier\RCS_NLP\Research_Case_Agent_Modeling\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABA79900-E866-41CB-8CC6-0343AC2DF592}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA66627-1E85-4B83-BCB6-906D7F94BF89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{9415CE1A-2F07-42CD-B621-6EB7C8B55F7A}"/>
   </bookViews>
@@ -1984,7 +1984,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A144" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D152" sqref="D152"/>
+      <selection pane="bottomLeft" activeCell="E149" sqref="E149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4612,7 +4612,7 @@
         <v>432</v>
       </c>
       <c r="E148" t="s">
-        <v>185</v>
+        <v>457</v>
       </c>
       <c r="F148" t="s">
         <v>441</v>

</xml_diff>